<commit_message>
Commit related to Excel - read
</commit_message>
<xml_diff>
--- a/src/main/java/ExcelReadUtil/MmtTestData.xlsx
+++ b/src/main/java/ExcelReadUtil/MmtTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B186B5EF-F3C8-44F9-BA45-F33A1DCCDE2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{21C57298-24C8-4FF1-9FB4-FB2541B0B880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="1280" windowWidth="15400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="2076" windowWidth="11100" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
-    <t>Headers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flights, Hotels, Villas &amp; Apts, Holidays, Trains, Buses, Visa, Cabs, Charter Flights, </t>
+    <t>Rahul Shetty Academy</t>
   </si>
 </sst>
 </file>
@@ -42,12 +39,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -355,23 +350,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>